<commit_message>
RTI Scenario 5 Code Changes-16-10-2017
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400"/>
+    <workbookView activeTab="10" firstSheet="8" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForJan" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="49" r:id="rId5"/>
-    <sheet name="TestJanReports" sheetId="11" r:id="rId6"/>
-    <sheet name="ResetEmployeeData12" sheetId="113" r:id="rId7"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="67" r:id="rId8"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="68" r:id="rId9"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="69" r:id="rId10"/>
-    <sheet name="TestMarchReports" sheetId="70" r:id="rId11"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId5" sheetId="49"/>
+    <sheet name="TestJanReports" r:id="rId6" sheetId="11"/>
+    <sheet name="ResetEmployeeData12" r:id="rId7" sheetId="113"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId8" sheetId="67"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId9" sheetId="68"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId10" sheetId="69"/>
+    <sheet name="TestMarchReports" r:id="rId11" sheetId="70"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="71">
   <si>
     <t>TC</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>DONT TOUCH AUTO EMPLR HMRC RECNTION</t>
-  </si>
-  <si>
-    <t>5</t>
   </si>
   <si>
     <t>ExpectedResultRowNumOfTestResultFile</t>
@@ -215,9 +212,6 @@
     <t>DO NOT TOUCH PAYROL RTI SCENRIO5 REPORT</t>
   </si>
   <si>
-    <t>Jan-2017</t>
-  </si>
-  <si>
     <t>Robin/2</t>
   </si>
   <si>
@@ -237,13 +231,26 @@
   </si>
   <si>
     <t>ResetEmployeeData12</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>January-2018</t>
+  </si>
+  <si>
+    <t>March-2018-Final</t>
+  </si>
+  <si>
+    <t>11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -274,6 +281,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -317,69 +330,70 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="21">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="2">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -396,10 +410,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -434,7 +448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -486,7 +500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -591,7 +605,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -600,13 +614,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -616,7 +630,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -625,7 +639,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -634,7 +648,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -644,12 +658,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -680,7 +694,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -699,7 +713,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -711,19 +725,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:D7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,7 +756,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>28</v>
@@ -756,7 +770,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>28</v>
@@ -770,7 +784,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>28</v>
@@ -784,7 +798,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="13" t="s">
         <v>28</v>
@@ -798,7 +812,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>28</v>
@@ -812,7 +826,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>28</v>
@@ -826,7 +840,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>28</v>
@@ -840,7 +854,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>28</v>
@@ -854,7 +868,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>28</v>
@@ -868,7 +882,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B11" s="13" t="s">
         <v>28</v>
@@ -1041,12 +1055,12 @@
       <c r="C51" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1055,20 +1069,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1115,33 +1129,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>23</v>
@@ -1156,36 +1170,36 @@
       <c r="N2" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="22.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45.75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
@@ -1220,13 +1234,13 @@
         <v>24</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>33</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>2</v>
@@ -1238,33 +1252,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>64</v>
+      <c r="E2" s="20" t="s">
+        <v>69</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="17" t="s">
         <v>65</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>23</v>
@@ -1272,9 +1286,15 @@
       <c r="K2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="L2" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="O2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1282,24 +1302,24 @@
       <c r="Q2" s="19"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1307,13 +1327,13 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -1325,12 +1345,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>13</v>
@@ -1345,13 +1365,13 @@
       <c r="G2" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1360,10 +1380,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1395,18 +1415,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="9" t="s">
         <v>56</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>57</v>
       </c>
       <c r="E2" s="10">
         <v>30000</v>
@@ -1421,13 +1441,13 @@
       <c r="I2" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1436,18 +1456,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.42578125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1494,30 +1514,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>25</v>
@@ -1535,13 +1555,13 @@
       <c r="N2" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1550,18 +1570,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1608,30 +1628,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="7" t="s">
         <v>26</v>
@@ -1649,37 +1669,37 @@
       <c r="N2" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.7109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
@@ -1714,13 +1734,13 @@
         <v>24</v>
       </c>
       <c r="L1" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="N1" s="16" t="s">
         <v>32</v>
-      </c>
-      <c r="N1" s="16" t="s">
-        <v>33</v>
       </c>
       <c r="O1" s="16" t="s">
         <v>2</v>
@@ -1732,33 +1752,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>60</v>
-      </c>
       <c r="H2" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="17" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J2" s="17" t="s">
         <v>23</v>
@@ -1766,9 +1786,15 @@
       <c r="K2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
+      <c r="L2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="O2" s="19" t="s">
         <v>4</v>
       </c>
@@ -1776,13 +1802,13 @@
       <c r="Q2" s="19"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1791,13 +1817,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1805,13 +1831,13 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>37</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>2</v>
@@ -1823,12 +1849,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="89.25" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="17" t="s">
         <v>13</v>
@@ -1843,12 +1869,12 @@
       <c r="G2" s="18"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1857,15 +1883,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" customWidth="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1897,18 +1923,18 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="84" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="10">
         <v>30000</v>
@@ -1923,12 +1949,12 @@
       <c r="I2" s="8"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1937,20 +1963,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.28515625" customWidth="1"/>
-    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1997,33 +2023,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I2" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="7" t="s">
         <v>23</v>
@@ -2038,6 +2064,6 @@
       <c r="N2" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
RTI Scenario5 Code Checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="70">
   <si>
     <t>TC</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>March-2018-Final</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
 </sst>
 </file>
@@ -250,7 +247,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -281,12 +278,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -385,7 +376,9 @@
     <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
@@ -1178,8 +1171,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1189,8 +1182,8 @@
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.42578125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
@@ -1256,8 +1249,8 @@
       <c r="A2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>64</v>
+      <c r="B2" s="20" t="s">
+        <v>61</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>38</v>
@@ -1265,7 +1258,7 @@
       <c r="D2" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="17" t="s">
         <v>69</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -1287,13 +1280,13 @@
         <v>26</v>
       </c>
       <c r="L2" s="17" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="M2" s="17" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="O2" s="19" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
updated RTI 5,6 and 7 Scenarios input sheet
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
@@ -1,35 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="5" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
+    <workbookView xWindow="396" yWindow="36" windowWidth="15168" windowHeight="5400" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId3" sheetId="6"/>
-    <sheet name="ProcessPayrollForJan" r:id="rId4" sheetId="7"/>
-    <sheet name="ProcessFinalPayrollForJan" r:id="rId5" sheetId="49"/>
-    <sheet name="TestJanReports" r:id="rId6" sheetId="11"/>
-    <sheet name="ResetEmployeeData12" r:id="rId7" sheetId="113"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId8" sheetId="67"/>
-    <sheet name="ProcessPayrollForMarch" r:id="rId9" sheetId="68"/>
-    <sheet name="ProcessFinalPayrollForMarch" r:id="rId10" sheetId="69"/>
-    <sheet name="TestMarchReports" r:id="rId11" sheetId="70"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="6" r:id="rId3"/>
+    <sheet name="ProcessPayrollForJan" sheetId="7" r:id="rId4"/>
+    <sheet name="ProcessFinalPayrollForJan" sheetId="49" r:id="rId5"/>
+    <sheet name="TestJanReports" sheetId="11" r:id="rId6"/>
+    <sheet name="ResetEmployeeData12" sheetId="113" r:id="rId7"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="67" r:id="rId8"/>
+    <sheet name="ProcessPayrollForMarch" sheetId="68" r:id="rId9"/>
+    <sheet name="ProcessFinalPayrollForMarch" sheetId="69" r:id="rId10"/>
+    <sheet name="TestMarchReports" sheetId="70" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
   <si>
     <t>TC</t>
   </si>
@@ -118,9 +113,6 @@
     <t>dd</t>
   </si>
   <si>
-    <t>DONT TOUCH AUTO EMPLR HMRC RECNTION</t>
-  </si>
-  <si>
     <t>ExpectedResultRowNumOfTestResultFile</t>
   </si>
   <si>
@@ -143,9 +135,6 @@
   </si>
   <si>
     <t>A All other employees</t>
-  </si>
-  <si>
-    <t>Monthly_RTIPayroll</t>
   </si>
   <si>
     <t xml:space="preserve">F:\\Automation_TestResults\\Payroll_Tax_RTI_TestReports201718\\201718 Payroll RTI Recognition Test result.xlsx
@@ -237,14 +226,19 @@
   </si>
   <si>
     <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE Rejoiner 105</t>
+  </si>
+  <si>
+    <t>DONT TOUCH AUTO HMRCS5 EMPLOYER</t>
+  </si>
+  <si>
+    <t>HMRCS5_Payroll</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,14 +250,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -317,72 +303,67 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+  <cellXfs count="19">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="2">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="3" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -399,10 +380,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -437,7 +418,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,26 +451,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -522,23 +486,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -594,7 +541,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -603,13 +550,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -619,7 +566,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -628,7 +575,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -637,7 +584,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -647,12 +594,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -683,7 +630,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -702,7 +649,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -714,22 +661,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -743,11 +690,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C2" s="9" t="s">
@@ -757,11 +704,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C3" s="9" t="s">
@@ -771,11 +718,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -785,11 +732,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -799,11 +746,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -813,11 +760,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -827,11 +774,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -841,11 +788,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -855,11 +802,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -869,11 +816,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>28</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -883,198 +830,198 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1118,33 +1065,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
+    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>40</v>
+        <v>56</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>23</v>
@@ -1152,177 +1099,177 @@
       <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="2" max="2" width="22.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.88671875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.44140625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="45.75" r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="19" t="s">
+    <row r="2" spans="1:17" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="J2" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="16" t="s">
+      <c r="M2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="34.109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.88671875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1334,48 +1281,48 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>54</v>
+    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C2" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" width="32.5546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1404,18 +1351,18 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E2" s="9">
         <v>30000</v>
@@ -1430,36 +1377,36 @@
       <c r="I2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1503,30 +1450,30 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>39</v>
+      <c r="H2" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>25</v>
@@ -1537,43 +1484,43 @@
       <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.44140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.88671875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1617,30 +1564,30 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>40</v>
+      <c r="H2" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>26</v>
@@ -1651,182 +1598,182 @@
       <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.6640625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="35" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="32.6640625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="33.33203125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="30" r="1" s="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="O1" s="15" t="s">
+      <c r="O1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="15" t="s">
+      <c r="P1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="Q1" s="15" t="s">
+      <c r="Q1" s="14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="7" t="s">
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" s="16" t="s">
+      <c r="L2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="18" t="s">
+      <c r="O2" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="18"/>
-      <c r="Q2" s="18"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.44140625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="5" t="s">
         <v>35</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>36</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1838,52 +1785,52 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="89.25" r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="16" t="s">
-        <v>68</v>
+    <row r="2" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17" t="s">
+      <c r="E2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="20.33203125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1912,18 +1859,18 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="84" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E2" s="9">
         <v>30000</v>
@@ -1938,37 +1885,37 @@
       <c r="I2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.33203125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -2012,33 +1959,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>29</v>
+    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>38</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>39</v>
+        <v>56</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>37</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>23</v>
@@ -2046,13 +1993,13 @@
       <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="14"/>
-      <c r="N2" s="14"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
XML File name change for Tax module as per Jenkisn Job creation.
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
@@ -4,27 +4,27 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="396" yWindow="36" windowWidth="15168" windowHeight="5400" firstSheet="6" activeTab="8"/>
+    <workbookView activeTab="8" firstSheet="6" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
   </bookViews>
   <sheets>
-    <sheet name="first" sheetId="1" r:id="rId1"/>
-    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="6" r:id="rId3"/>
-    <sheet name="ProcessPayrollForJan" sheetId="7" r:id="rId4"/>
-    <sheet name="ProcessFinalPayrollForJan" sheetId="49" r:id="rId5"/>
-    <sheet name="TestJanReports" sheetId="11" r:id="rId6"/>
-    <sheet name="ResetEmployeeData12" sheetId="113" r:id="rId7"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="67" r:id="rId8"/>
-    <sheet name="ProcessPayrollForMarch" sheetId="68" r:id="rId9"/>
-    <sheet name="ProcessFinalPayrollForMarch" sheetId="69" r:id="rId10"/>
-    <sheet name="TestMarchReports" sheetId="70" r:id="rId11"/>
+    <sheet name="first" r:id="rId1" sheetId="1"/>
+    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId3" sheetId="6"/>
+    <sheet name="ProcessPayrollForJan" r:id="rId4" sheetId="7"/>
+    <sheet name="ProcessFinalPayrollForJan" r:id="rId5" sheetId="49"/>
+    <sheet name="TestJanReports" r:id="rId6" sheetId="11"/>
+    <sheet name="ResetEmployeeData12" r:id="rId7" sheetId="113"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId8" sheetId="67"/>
+    <sheet name="ProcessPayrollForMarch" r:id="rId9" sheetId="68"/>
+    <sheet name="ProcessFinalPayrollForMarch" r:id="rId10" sheetId="69"/>
+    <sheet name="TestMarchReports" r:id="rId11" sheetId="70"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="69">
   <si>
     <t>TC</t>
   </si>
@@ -238,6 +238,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -304,66 +305,66 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -380,10 +381,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -541,7 +542,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -550,13 +551,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -566,7 +567,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -575,7 +576,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -584,7 +585,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -594,12 +595,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -630,7 +631,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -649,7 +650,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -661,7 +662,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -670,13 +671,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -690,7 +691,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -704,7 +705,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>43</v>
       </c>
@@ -718,7 +719,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>44</v>
       </c>
@@ -732,7 +733,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>45</v>
       </c>
@@ -746,7 +747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>46</v>
       </c>
@@ -760,7 +761,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>62</v>
       </c>
@@ -774,7 +775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>47</v>
       </c>
@@ -788,7 +789,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>48</v>
       </c>
@@ -802,7 +803,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>49</v>
       </c>
@@ -816,7 +817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>50</v>
       </c>
@@ -830,35 +831,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
     </row>
-    <row r="19" spans="2:3" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
     </row>
@@ -991,12 +992,12 @@
       <c r="C51" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1005,23 +1006,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="22.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1065,7 +1066,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -1106,12 +1107,12 @@
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1120,22 +1121,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.88671875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="29.44140625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.88671875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.44140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="45.75" r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1188,7 +1189,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="125.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -1238,12 +1239,12 @@
       <c r="Q2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1252,13 +1253,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.109375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.88671875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="34.109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>52</v>
       </c>
@@ -1301,13 +1302,13 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1316,13 +1317,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.88671875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>39</v>
       </c>
@@ -1377,13 +1378,13 @@
       <c r="I2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1392,18 +1393,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.44140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="18.5546875" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.109375" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="46.5546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.88671875" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.5546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.6640625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -1450,7 +1451,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -1491,13 +1492,13 @@
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1506,21 +1507,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="22.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="26.44140625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="41.88671875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.33203125" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.33203125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.88671875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1564,7 +1565,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -1605,37 +1606,37 @@
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView workbookViewId="0" zoomScaleNormal="100">
       <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="30.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="37.6640625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="43.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="22.33203125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="35" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="32.6640625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="33.33203125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.6640625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.6640625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row customFormat="1" ht="30" r="1" s="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1688,7 +1689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="4" customFormat="1" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -1738,13 +1739,13 @@
       <c r="Q2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1753,16 +1754,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.6640625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="6.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.44140625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="25.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.88671875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.88671875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="6.44140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.6640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1785,7 +1786,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="89.25" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>66</v>
       </c>
@@ -1805,12 +1806,12 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1819,18 +1820,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1859,7 +1860,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
+    <row customHeight="1" ht="84" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>66</v>
       </c>
@@ -1885,12 +1886,12 @@
       <c r="I2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -1899,23 +1900,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="18.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="28.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="27.33203125" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="23.44140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="4.88671875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.44140625" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="18" t="s">
         <v>67</v>
       </c>
@@ -2000,6 +2001,6 @@
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Out Put HTML files checkin
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="6" windowHeight="5400" windowWidth="15168" xWindow="396" yWindow="36"/>
+    <workbookView activeTab="10" firstSheet="8" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
   </bookViews>
   <sheets>
     <sheet name="first" r:id="rId1" sheetId="1"/>
@@ -24,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="66">
   <si>
     <t>TC</t>
   </si>
@@ -144,9 +149,6 @@
     <t>F:\\Automation_TestResults\\Payroll_Tax_RTI_TestReports201718\\201718 Payroll RTI Recognition Test result.xlsx</t>
   </si>
   <si>
-    <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 107</t>
-  </si>
-  <si>
     <t>Month 1</t>
   </si>
   <si>
@@ -183,18 +185,12 @@
     <t>Robin/1</t>
   </si>
   <si>
-    <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 105</t>
-  </si>
-  <si>
     <t>1150L</t>
   </si>
   <si>
     <t>Cumulative</t>
   </si>
   <si>
-    <t>Jan-2018</t>
-  </si>
-  <si>
     <t>Payroll Recognition ScenarioFive201718.xlsx</t>
   </si>
   <si>
@@ -204,9 +200,6 @@
     <t>Robin/2</t>
   </si>
   <si>
-    <t>March-2018</t>
-  </si>
-  <si>
     <t>DO NOT TOUCH PAYROL RTI SCENRIO5 REJOIN</t>
   </si>
   <si>
@@ -232,12 +225,15 @@
   </si>
   <si>
     <t>HMRCS5_Payroll</t>
+  </si>
+  <si>
+    <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -419,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -452,9 +448,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -487,6 +500,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -669,15 +699,15 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -691,7 +721,7 @@
         <v>3</v>
       </c>
     </row>
-    <row ht="15" r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>32</v>
       </c>
@@ -705,9 +735,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>28</v>
@@ -719,9 +749,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>28</v>
@@ -733,9 +763,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>28</v>
@@ -747,9 +777,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>28</v>
@@ -761,9 +791,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>28</v>
@@ -775,9 +805,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>28</v>
@@ -789,9 +819,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>28</v>
@@ -803,9 +833,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>28</v>
@@ -817,9 +847,9 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>28</v>
@@ -831,163 +861,163 @@
         <v>5</v>
       </c>
     </row>
-    <row ht="15" r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="1"/>
     </row>
-    <row ht="15" r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="1"/>
     </row>
-    <row ht="15" r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="1"/>
     </row>
-    <row ht="15" r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="1"/>
     </row>
-    <row ht="15" r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="1"/>
     </row>
-    <row ht="15" r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="1"/>
     </row>
-    <row ht="15" r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="1"/>
     </row>
-    <row ht="15" r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="1"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="1"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="1"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="1"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="1"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="1"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="2"/>
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="2"/>
       <c r="C35" s="1"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="2"/>
       <c r="C36" s="1"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="C37" s="1"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="2"/>
       <c r="C38" s="1"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
       <c r="C39" s="1"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="2"/>
       <c r="C40" s="1"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="2"/>
       <c r="C41" s="1"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="2"/>
       <c r="C42" s="1"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="2"/>
       <c r="C43" s="1"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="2"/>
       <c r="C44" s="1"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
       <c r="C45" s="1"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="2"/>
       <c r="C46" s="1"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="2"/>
       <c r="C47" s="1"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="2"/>
       <c r="C48" s="1"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="2"/>
       <c r="C49" s="1"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="2"/>
       <c r="C50" s="1"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="2"/>
       <c r="C51" s="1"/>
     </row>
@@ -1001,28 +1031,28 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1066,33 +1096,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>59</v>
+      <c r="E2" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>23</v>
@@ -1115,25 +1145,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.88671875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.44140625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.88671875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.6640625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customHeight="1" ht="45.75" r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -1189,33 +1219,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>38</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="J2" s="15" t="s">
         <v>23</v>
@@ -1224,7 +1254,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>25</v>
@@ -1248,18 +1278,18 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1284,10 +1314,10 @@
     </row>
     <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>13</v>
@@ -1312,18 +1342,18 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.5546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1354,16 +1384,16 @@
     </row>
     <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>39</v>
+        <v>65</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E2" s="9">
         <v>30000</v>
@@ -1388,26 +1418,26 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="31.6640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.44140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.44140625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.5546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.88671875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5546875" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.5546875" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.109375" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1451,27 +1481,27 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>37</v>
@@ -1502,26 +1532,26 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.33203125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.44140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="41.88671875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.33203125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.6640625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1565,27 +1595,27 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="55.95" r="2" s="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>38</v>
@@ -1615,25 +1645,25 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.33203125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.33203125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.6640625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="43.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
     <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.44140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.33203125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
     <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="32.6640625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="33.33203125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row customFormat="1" ht="30" r="1" s="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -1689,27 +1719,27 @@
         <v>7</v>
       </c>
     </row>
-    <row customFormat="1" customHeight="1" ht="62.4" r="2" s="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>38</v>
@@ -1724,7 +1754,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="M2" s="15" t="s">
         <v>25</v>
@@ -1752,18 +1782,18 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="25.6640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.88671875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.88671875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.88671875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="6.44140625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.6640625" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1788,10 +1818,10 @@
     </row>
     <row customHeight="1" ht="89.25" r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C2" s="15" t="s">
         <v>13</v>
@@ -1818,20 +1848,20 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>9</v>
       </c>
@@ -1862,16 +1892,16 @@
     </row>
     <row customHeight="1" ht="84" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>36</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="9">
         <v>30000</v>
@@ -1894,29 +1924,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.88671875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
     <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="27.33203125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.109375" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.44140625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5546875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="4.88671875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="5.33203125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="27.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="15" r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>14</v>
       </c>
@@ -1960,33 +1990,33 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>59</v>
+      <c r="E2" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>60</v>
       </c>
       <c r="H2" s="11" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" s="6" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
RTI 7 Scenarios input files checkin for employee changes
</commit_message>
<xml_diff>
--- a/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
+++ b/Salesforce_Core_Framework/src/main/java/com/test/xcdhr/Salesforce_Core_Framework1/salesforce_XLS_Files/Payroll Recognition ScenarioFive201718.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\XCDHR\git\XCDHR_Payroll\Salesforce_Core_Framework\src\main\java\com\test\xcdhr\Salesforce_Core_Framework1\salesforce_XLS_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView activeTab="10" firstSheet="8" windowHeight="5400" windowWidth="15165" xWindow="390" yWindow="30"/>
+    <workbookView xWindow="390" yWindow="30" windowWidth="15165" windowHeight="5400" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
-    <sheet name="first" r:id="rId1" sheetId="1"/>
-    <sheet name="ResetEmployeeData" r:id="rId2" sheetId="14"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM10" r:id="rId3" sheetId="6"/>
-    <sheet name="ProcessPayrollForJan" r:id="rId4" sheetId="7"/>
-    <sheet name="ProcessFinalPayrollForJan" r:id="rId5" sheetId="49"/>
-    <sheet name="TestJanReports" r:id="rId6" sheetId="11"/>
-    <sheet name="ResetEmployeeData12" r:id="rId7" sheetId="113"/>
-    <sheet name="UpdteTaxCodeAndAnualSalaryM12" r:id="rId8" sheetId="67"/>
-    <sheet name="ProcessPayrollForMarch" r:id="rId9" sheetId="68"/>
-    <sheet name="ProcessFinalPayrollForMarch" r:id="rId10" sheetId="69"/>
-    <sheet name="TestMarchReports" r:id="rId11" sheetId="70"/>
+    <sheet name="first" sheetId="1" r:id="rId1"/>
+    <sheet name="ResetEmployeeData" sheetId="14" r:id="rId2"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM10" sheetId="6" r:id="rId3"/>
+    <sheet name="ProcessPayrollForJan" sheetId="7" r:id="rId4"/>
+    <sheet name="ProcessFinalPayrollForJan" sheetId="49" r:id="rId5"/>
+    <sheet name="TestJanReports" sheetId="11" r:id="rId6"/>
+    <sheet name="ResetEmployeeData12" sheetId="113" r:id="rId7"/>
+    <sheet name="UpdteTaxCodeAndAnualSalaryM12" sheetId="67" r:id="rId8"/>
+    <sheet name="ProcessPayrollForMarch" sheetId="68" r:id="rId9"/>
+    <sheet name="ProcessFinalPayrollForMarch" sheetId="69" r:id="rId10"/>
+    <sheet name="TestMarchReports" sheetId="70" r:id="rId11"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="66">
   <si>
     <t>TC</t>
   </si>
@@ -227,14 +227,14 @@
     <t>HMRCS5_Payroll</t>
   </si>
   <si>
-    <t>DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 5</t>
+    <t xml:space="preserve">
+DO NOT TOUCH AUTOMATION HMRC RECOGNITION EMPLOYEE 105</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,66 +301,66 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="2" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -377,10 +377,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -415,7 +415,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -467,7 +467,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -572,7 +572,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -581,13 +581,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -597,7 +597,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -606,7 +606,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -615,7 +615,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -625,12 +625,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -661,7 +661,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -680,7 +680,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -692,7 +692,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -701,10 +701,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
+    <col min="1" max="1" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,12 +1022,12 @@
       <c r="C51" s="1"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1036,20 +1036,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="23.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1096,7 +1096,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>63</v>
       </c>
@@ -1137,36 +1137,36 @@
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="29.42578125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="2" max="2" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="29.42578125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="45.75" r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>14</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="125.25" r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="125.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>63</v>
       </c>
@@ -1269,24 +1269,24 @@
       <c r="Q2" s="17"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="34.140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="8.140625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="1" max="1" width="40.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -1312,7 +1312,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>65</v>
       </c>
@@ -1332,13 +1332,516 @@
       <c r="G2" s="16"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.5703125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="E2" s="9">
+        <v>30000</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="18.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.140625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="46.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="26.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="41.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="3" customFormat="1" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="30.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="37.7109375" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="43.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="35" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="32.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="33.28515625" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q1" s="14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" s="4" customFormat="1" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H2" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1347,10 +1850,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="32.5703125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="1" max="1" width="20.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1382,9 +1890,9 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="84" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>36</v>
@@ -1393,7 +1901,7 @@
         <v>51</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E2" s="9">
         <v>30000</v>
@@ -1408,520 +1916,12 @@
       <c r="I2" s="7"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="31.7109375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="46.5703125" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="12.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="23.5703125" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="11.140625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup horizontalDpi="0" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="32.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="34.28515625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="26.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="41.85546875" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="12.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="55.9" r="2" s="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="32.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="30.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="43.28515625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="11.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="22.28515625" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="35.0" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="32.7109375" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="33.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row customFormat="1" ht="30" r="1" s="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customFormat="1" customHeight="1" ht="62.45" r="2" s="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="C2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="N2" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="25.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.85546875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="6.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="9.7109375" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="89.25" r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row customHeight="1" ht="84" r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E2" s="9">
-        <v>30000</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-    </row>
-  </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1930,20 +1930,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="28.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="4.85546875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="5.28515625" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="21" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="28.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="27.28515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="11.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="9.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="4.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="5.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
         <v>7</v>
       </c>
     </row>
-    <row customHeight="1" ht="86.25" r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
         <v>63</v>
       </c>
@@ -2031,6 +2031,6 @@
       <c r="N2" s="13"/>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>